<commit_message>
23.05.06 Fix kg_scef_tidy command
</commit_message>
<xml_diff>
--- a/ExsampleData/Test_Shortcut_data.xlsx
+++ b/ExsampleData/Test_Shortcut_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R_create_package\KG_Loupedeck\KGLoupedeck\ExsampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6041A7EC-110B-41D5-85FD-2243B4492BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1491D3EB-BCFD-41BA-B980-3E92A8CFC8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23925" yWindow="4275" windowWidth="25425" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27360" yWindow="1950" windowWidth="25425" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,9 +82,6 @@
     <t>Main Menu (Server)</t>
   </si>
   <si>
-    <t>Help Menu</t>
-  </si>
-  <si>
     <t>Alt+Shift+H</t>
   </si>
   <si>
@@ -103,6 +100,10 @@
   <si>
     <t>Icon_Text_Color</t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>help menu</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -214,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -250,9 +251,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -545,7 +543,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -563,10 +561,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -614,7 +612,7 @@
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="8"/>
       <c r="D4" s="3" t="s">
         <v>13</v>
@@ -633,13 +631,13 @@
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -649,13 +647,13 @@
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
23.05.07 Fix kg_scef_tidy command
</commit_message>
<xml_diff>
--- a/ExsampleData/Test_Shortcut_data.xlsx
+++ b/ExsampleData/Test_Shortcut_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R_create_package\KG_Loupedeck\KGLoupedeck\ExsampleData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1491D3EB-BCFD-41BA-B980-3E92A8CFC8CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E305139-A9F0-4379-B3D5-3E7E07F5CB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27360" yWindow="1950" windowWidth="25425" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-615" yWindow="1560" windowWidth="25425" windowHeight="13725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,16 +73,10 @@
     <t>Diff active source document</t>
   </si>
   <si>
-    <t>Ctrl+Alt+D</t>
-  </si>
-  <si>
     <t>Ctrl+Option+D</t>
   </si>
   <si>
     <t>Main Menu (Server)</t>
-  </si>
-  <si>
-    <t>Alt+Shift+H</t>
   </si>
   <si>
     <t>Ctrl+Option+H</t>
@@ -103,6 +97,14 @@
   </si>
   <si>
     <t>help menu</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Ctrl+Alt+D</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Alt+Shift+H</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -261,6 +263,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99CC00"/>
       <color rgb="FF1EC031"/>
       <color rgb="FF6B3E1D"/>
       <color rgb="FFCB39A1"/>
@@ -543,7 +546,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -551,8 +554,8 @@
     <col min="1" max="1" width="28.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.5" customWidth="1"/>
     <col min="6" max="6" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -561,10 +564,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>1</v>
@@ -618,26 +621,26 @@
         <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -647,13 +650,13 @@
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>